<commit_message>
fixed arabic charts section
</commit_message>
<xml_diff>
--- a/data/AR_DATA.xlsx
+++ b/data/AR_DATA.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="135" windowWidth="10500" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="9855" yWindow="135" windowWidth="10500" windowHeight="7935"/>
   </bookViews>
   <sheets>
-    <sheet name="RESULTS" sheetId="1" r:id="rId1"/>
-    <sheet name="ELECTION DATA" sheetId="2" r:id="rId2"/>
-    <sheet name="INS DATA" sheetId="3" r:id="rId3"/>
-    <sheet name="POLLING DATA" sheetId="4" r:id="rId4"/>
+    <sheet name="نتائج الأحزاب" sheetId="1" r:id="rId1"/>
+    <sheet name="معطيات إنتخابية" sheetId="2" r:id="rId2"/>
+    <sheet name="معطيات إجتماعية و إقتصادية" sheetId="3" r:id="rId3"/>
+    <sheet name="معطيات الاقتراع" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -19,179 +19,179 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
   <si>
-    <t>Electoral District</t>
-  </si>
-  <si>
-    <t>NAHDHA</t>
-  </si>
-  <si>
-    <t>ARIDHA</t>
-  </si>
-  <si>
-    <t>ETTAKATOL</t>
-  </si>
-  <si>
-    <t>CPR</t>
-  </si>
-  <si>
-    <t>PDP</t>
-  </si>
-  <si>
-    <t>Eligible Voters</t>
-  </si>
-  <si>
-    <t>Blank Ballots</t>
-  </si>
-  <si>
-    <t>Cancelled Ballots</t>
-  </si>
-  <si>
-    <t>Wasted Ballots</t>
-  </si>
-  <si>
-    <t>Actively Registered Ratio</t>
-  </si>
-  <si>
-    <t>Passively Registered Ratio</t>
-  </si>
-  <si>
-    <t>Actively Registered Turnout</t>
-  </si>
-  <si>
-    <t>Passively Registered Turnout</t>
-  </si>
-  <si>
-    <t>Youth Ratio</t>
-  </si>
-  <si>
-    <t>Mobile Coverage</t>
-  </si>
-  <si>
-    <t>Computer Coverage</t>
-  </si>
-  <si>
-    <t>Internet Coverage</t>
-  </si>
-  <si>
-    <t>Unemployment Ratio</t>
-  </si>
-  <si>
-    <t>Illetracy Ratio</t>
-  </si>
-  <si>
-    <t>Higher Education Ratio</t>
-  </si>
-  <si>
-    <t>Turnout</t>
-  </si>
-  <si>
-    <t>Tunis 1</t>
-  </si>
-  <si>
-    <t>Tunis 2</t>
-  </si>
-  <si>
-    <t>Ariana</t>
-  </si>
-  <si>
-    <t>Ben Arous</t>
-  </si>
-  <si>
-    <t>Manouba</t>
-  </si>
-  <si>
-    <t>Nabeul 1</t>
-  </si>
-  <si>
-    <t>Nabeul 2</t>
-  </si>
-  <si>
-    <t>Zaghouan</t>
-  </si>
-  <si>
-    <t>Bizerte</t>
-  </si>
-  <si>
-    <t>Beja</t>
-  </si>
-  <si>
-    <t>Jendouba</t>
-  </si>
-  <si>
-    <t>Kef</t>
-  </si>
-  <si>
-    <t>Siliana</t>
-  </si>
-  <si>
-    <t>Sousse</t>
-  </si>
-  <si>
-    <t>Monastir</t>
-  </si>
-  <si>
-    <t>Mahdia</t>
-  </si>
-  <si>
-    <t>Sfax 1</t>
-  </si>
-  <si>
-    <t>Sfax 2</t>
-  </si>
-  <si>
-    <t>Kairouan</t>
-  </si>
-  <si>
-    <t>Kasserine</t>
-  </si>
-  <si>
-    <t>Sidi Bouzid</t>
-  </si>
-  <si>
-    <t>Gabes</t>
-  </si>
-  <si>
-    <t>Medenine</t>
-  </si>
-  <si>
-    <t>Tataouine</t>
-  </si>
-  <si>
-    <t>Gafsa</t>
-  </si>
-  <si>
-    <t>Tozeur</t>
-  </si>
-  <si>
-    <t>Kebili</t>
-  </si>
-  <si>
-    <t>District_ID</t>
-  </si>
-  <si>
-    <t>Number of electoral lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of pollworkers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Education Ratio </t>
-  </si>
-  <si>
-    <t>% of unemployed with higher education</t>
-  </si>
-  <si>
-    <t>AFEK TOUNES</t>
-  </si>
-  <si>
-    <t>Number of polling stations</t>
+    <t>النهضة</t>
+  </si>
+  <si>
+    <t>العريضة الشعبية</t>
+  </si>
+  <si>
+    <t>التكتل</t>
+  </si>
+  <si>
+    <t>المؤتمر من أجل الجمهورية</t>
+  </si>
+  <si>
+    <t>الحزب الديمقراطي التقدمي</t>
+  </si>
+  <si>
+    <t>أفاق تونس</t>
+  </si>
+  <si>
+    <t>الناخبين المحتملين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أوراق الاقتراع البيضاء </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الأوراق الملغاة </t>
+  </si>
+  <si>
+    <t>أوراق الاقتراع  الضائعة</t>
+  </si>
+  <si>
+    <t>نسبة المسجلين إراديا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نسبة المسجلين آليا </t>
+  </si>
+  <si>
+    <t>نسبة الشباب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تغطية الهاتف الجوال </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تغطية الحواسيب </t>
+  </si>
+  <si>
+    <t>الوصول إلى الإنترنت</t>
+  </si>
+  <si>
+    <t>نسبة الأمية</t>
+  </si>
+  <si>
+    <t>نسبة البطالة</t>
+  </si>
+  <si>
+    <t>معدل خريجي التعليم العالي</t>
+  </si>
+  <si>
+    <t>معدل خريجي التعليم الثانوي</t>
+  </si>
+  <si>
+    <t>نسبة البطالة لخريجي  التعليم العالي</t>
+  </si>
+  <si>
+    <t>عدد القوائم الانتخابية</t>
+  </si>
+  <si>
+    <t>عدد العاملين في مراكز الاقتراع</t>
+  </si>
+  <si>
+    <t>عدد مكاتب الاقتراع</t>
+  </si>
+  <si>
+    <t>الدائرة الانتخابية</t>
+  </si>
+  <si>
+    <t>معرف الدائرة الانتخابية</t>
+  </si>
+  <si>
+    <t>نسبة المشاركة للمسجلين إراديا</t>
+  </si>
+  <si>
+    <t>نسبة المشاركة للمسجلين أليا</t>
+  </si>
+  <si>
+    <t>نسبة المشاركة</t>
+  </si>
+  <si>
+    <t>تونس 1</t>
+  </si>
+  <si>
+    <t>تونس 2</t>
+  </si>
+  <si>
+    <t>أريانة</t>
+  </si>
+  <si>
+    <t>بن عروس</t>
+  </si>
+  <si>
+    <t>منوبة</t>
+  </si>
+  <si>
+    <t>نابل 1</t>
+  </si>
+  <si>
+    <t>نابل 2</t>
+  </si>
+  <si>
+    <t>زغوان</t>
+  </si>
+  <si>
+    <t>بنزرت</t>
+  </si>
+  <si>
+    <t>باجة</t>
+  </si>
+  <si>
+    <t>جندوبة</t>
+  </si>
+  <si>
+    <t>الكاف</t>
+  </si>
+  <si>
+    <t>سليانـــة</t>
+  </si>
+  <si>
+    <t>سوسة</t>
+  </si>
+  <si>
+    <t>المنستير</t>
+  </si>
+  <si>
+    <t>المهدية</t>
+  </si>
+  <si>
+    <t>صفاقس 1</t>
+  </si>
+  <si>
+    <t>صفاقس 2</t>
+  </si>
+  <si>
+    <t>القيروان</t>
+  </si>
+  <si>
+    <t>القصرين</t>
+  </si>
+  <si>
+    <t>سيدي بوزيد</t>
+  </si>
+  <si>
+    <t>قابس</t>
+  </si>
+  <si>
+    <t>مدنين</t>
+  </si>
+  <si>
+    <t>تطاوين</t>
+  </si>
+  <si>
+    <t>قفصة</t>
+  </si>
+  <si>
+    <t>توزر</t>
+  </si>
+  <si>
+    <t>قبلي</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +333,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -677,7 +683,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -687,6 +693,11 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1032,48 +1043,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
+      <c r="B2" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="1">
         <v>0.4617</v>
@@ -1098,8 +1113,8 @@
       <c r="A3">
         <v>112</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
+      <c r="B3" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>0.30380000000000001</v>
@@ -1124,8 +1139,8 @@
       <c r="A4">
         <v>120</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
+      <c r="B4" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="1">
         <v>0.36130000000000001</v>
@@ -1150,8 +1165,8 @@
       <c r="A5">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
+      <c r="B5" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <v>0.4234</v>
@@ -1176,8 +1191,8 @@
       <c r="A6">
         <v>140</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
+      <c r="B6" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="1">
         <v>0.40679999999999999</v>
@@ -1202,8 +1217,8 @@
       <c r="A7">
         <v>151</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
+      <c r="B7" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="1">
         <v>0.31280000000000002</v>
@@ -1228,8 +1243,8 @@
       <c r="A8">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>0.29599999999999999</v>
@@ -1254,8 +1269,8 @@
       <c r="A9">
         <v>160</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="B9" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>0.34720000000000001</v>
@@ -1280,8 +1295,8 @@
       <c r="A10">
         <v>170</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
+      <c r="B10" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="1">
         <v>0.40989999999999999</v>
@@ -1306,8 +1321,8 @@
       <c r="A11">
         <v>210</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
+      <c r="B11" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>0.311</v>
@@ -1332,8 +1347,8 @@
       <c r="A12">
         <v>220</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
+      <c r="B12" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>0.28089999999999998</v>
@@ -1358,8 +1373,8 @@
       <c r="A13">
         <v>230</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
+      <c r="B13" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>0.26719999999999999</v>
@@ -1384,8 +1399,8 @@
       <c r="A14">
         <v>240</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="1">
         <v>0.28470000000000001</v>
@@ -1410,8 +1425,8 @@
       <c r="A15">
         <v>310</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
+      <c r="B15" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="1">
         <v>0.35849999999999999</v>
@@ -1436,8 +1451,8 @@
       <c r="A16">
         <v>320</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
+      <c r="B16" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="1">
         <v>0.3246</v>
@@ -1462,8 +1477,8 @@
       <c r="A17">
         <v>330</v>
       </c>
-      <c r="B17" t="s">
-        <v>37</v>
+      <c r="B17" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="1">
         <v>0.31080000000000002</v>
@@ -1488,8 +1503,8 @@
       <c r="A18">
         <v>341</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
+      <c r="B18" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="1">
         <v>0.44130000000000003</v>
@@ -1514,8 +1529,8 @@
       <c r="A19">
         <v>342</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
+      <c r="B19" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="1">
         <v>0.3785</v>
@@ -1540,8 +1555,8 @@
       <c r="A20">
         <v>410</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
+      <c r="B20" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C20" s="1">
         <v>0.42920000000000003</v>
@@ -1566,8 +1581,8 @@
       <c r="A21">
         <v>420</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
+      <c r="B21" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>0.31840000000000002</v>
@@ -1592,8 +1607,8 @@
       <c r="A22">
         <v>430</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
+      <c r="B22" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C22" s="1">
         <v>0.15579999999999999</v>
@@ -1618,8 +1633,8 @@
       <c r="A23">
         <v>510</v>
       </c>
-      <c r="B23" t="s">
-        <v>43</v>
+      <c r="B23" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C23" s="1">
         <v>0.53049999999999997</v>
@@ -1644,8 +1659,8 @@
       <c r="A24">
         <v>520</v>
       </c>
-      <c r="B24" t="s">
-        <v>44</v>
+      <c r="B24" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>0.4773</v>
@@ -1670,8 +1685,8 @@
       <c r="A25">
         <v>530</v>
       </c>
-      <c r="B25" t="s">
-        <v>45</v>
+      <c r="B25" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C25" s="1">
         <v>0.59379999999999999</v>
@@ -1696,8 +1711,8 @@
       <c r="A26">
         <v>610</v>
       </c>
-      <c r="B26" t="s">
-        <v>46</v>
+      <c r="B26" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C26" s="1">
         <v>0.40379999999999999</v>
@@ -1722,8 +1737,8 @@
       <c r="A27">
         <v>620</v>
       </c>
-      <c r="B27" t="s">
-        <v>47</v>
+      <c r="B27" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C27" s="1">
         <v>0.43090000000000001</v>
@@ -1748,8 +1763,8 @@
       <c r="A28">
         <v>630</v>
       </c>
-      <c r="B28" t="s">
-        <v>48</v>
+      <c r="B28" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C28" s="1">
         <v>0.40479999999999999</v>
@@ -1772,6 +1787,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1779,34 +1795,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1824,18 +1843,18 @@
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="1">
         <v>0.98089999999999999</v>
@@ -1869,8 +1888,8 @@
       <c r="A3">
         <v>112</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>0.75980000000000003</v>
@@ -1904,8 +1923,8 @@
       <c r="A4">
         <v>120</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="1">
         <v>0.74439999999999995</v>
@@ -1939,8 +1958,8 @@
       <c r="A5">
         <v>130</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <v>0.77510000000000001</v>
@@ -1974,8 +1993,8 @@
       <c r="A6">
         <v>140</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
+      <c r="B6" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="1">
         <v>0.73770000000000002</v>
@@ -2009,8 +2028,8 @@
       <c r="A7">
         <v>151</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="1">
         <v>0.88429999999999997</v>
@@ -2044,8 +2063,8 @@
       <c r="A8">
         <v>152</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>0.59079999999999999</v>
@@ -2079,8 +2098,8 @@
       <c r="A9">
         <v>160</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>0.76400000000000001</v>
@@ -2114,8 +2133,8 @@
       <c r="A10">
         <v>170</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>30</v>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="1">
         <v>0.82240000000000002</v>
@@ -2149,8 +2168,8 @@
       <c r="A11">
         <v>210</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>0.7853</v>
@@ -2184,8 +2203,8 @@
       <c r="A12">
         <v>220</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>0.78820000000000001</v>
@@ -2219,8 +2238,8 @@
       <c r="A13">
         <v>230</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
+      <c r="B13" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>0.80169999999999997</v>
@@ -2254,8 +2273,8 @@
       <c r="A14">
         <v>240</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="1">
         <v>0.76160000000000005</v>
@@ -2289,8 +2308,8 @@
       <c r="A15">
         <v>310</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="1">
         <v>0.76190000000000002</v>
@@ -2324,8 +2343,8 @@
       <c r="A16">
         <v>320</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>36</v>
+      <c r="B16" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="1">
         <v>0.72950000000000004</v>
@@ -2359,8 +2378,8 @@
       <c r="A17">
         <v>330</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
+      <c r="B17" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="1">
         <v>0.7329</v>
@@ -2394,8 +2413,8 @@
       <c r="A18">
         <v>341</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
+      <c r="B18" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="1">
         <v>0.55700000000000005</v>
@@ -2429,8 +2448,8 @@
       <c r="A19">
         <v>342</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
+      <c r="B19" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="1">
         <v>0.90669999999999995</v>
@@ -2464,8 +2483,8 @@
       <c r="A20">
         <v>410</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
+      <c r="B20" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="C20" s="1">
         <v>0.73560000000000003</v>
@@ -2499,8 +2518,8 @@
       <c r="A21">
         <v>420</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
+      <c r="B21" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>0.69220000000000004</v>
@@ -2534,8 +2553,8 @@
       <c r="A22">
         <v>430</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
+      <c r="B22" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C22" s="1">
         <v>0.75370000000000004</v>
@@ -2569,8 +2588,8 @@
       <c r="A23">
         <v>510</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
+      <c r="B23" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C23" s="1">
         <v>0.78</v>
@@ -2604,8 +2623,8 @@
       <c r="A24">
         <v>520</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
+      <c r="B24" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>0.83699999999999997</v>
@@ -2639,8 +2658,8 @@
       <c r="A25">
         <v>530</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
+      <c r="B25" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C25" s="1">
         <v>0.79730000000000001</v>
@@ -2674,8 +2693,8 @@
       <c r="A26">
         <v>610</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>46</v>
+      <c r="B26" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C26" s="1">
         <v>0.74960000000000004</v>
@@ -2709,8 +2728,8 @@
       <c r="A27">
         <v>620</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
+      <c r="B27" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="C27" s="1">
         <v>0.74750000000000005</v>
@@ -2744,8 +2763,8 @@
       <c r="A28">
         <v>630</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>48</v>
+      <c r="B28" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C28" s="1">
         <v>0.76290000000000002</v>
@@ -2788,7 +2807,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -2802,45 +2822,45 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="1">
         <v>0.36330000000000001</v>
@@ -2874,8 +2894,8 @@
       <c r="A3">
         <v>112</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>0.36330000000000001</v>
@@ -2909,8 +2929,8 @@
       <c r="A4">
         <v>120</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
+      <c r="B4" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="1">
         <v>0.37319999999999998</v>
@@ -2944,8 +2964,8 @@
       <c r="A5">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <v>0.36890000000000001</v>
@@ -2979,8 +2999,8 @@
       <c r="A6">
         <v>140</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
+      <c r="B6" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="1">
         <v>0.38279999999999997</v>
@@ -3014,8 +3034,8 @@
       <c r="A7">
         <v>151</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
+      <c r="B7" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="1">
         <v>0.36470000000000002</v>
@@ -3049,8 +3069,8 @@
       <c r="A8">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
+      <c r="B8" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>0.36470000000000002</v>
@@ -3084,8 +3104,8 @@
       <c r="A9">
         <v>160</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="B9" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>0.34250000000000003</v>
@@ -3119,8 +3139,8 @@
       <c r="A10">
         <v>170</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
+      <c r="B10" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="1">
         <v>0.37230000000000002</v>
@@ -3154,8 +3174,8 @@
       <c r="A11">
         <v>210</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>0.34110000000000001</v>
@@ -3189,8 +3209,8 @@
       <c r="A12">
         <v>220</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>0.3367</v>
@@ -3224,8 +3244,8 @@
       <c r="A13">
         <v>230</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
+      <c r="B13" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>0.3211</v>
@@ -3259,8 +3279,8 @@
       <c r="A14">
         <v>240</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="1">
         <v>0.3483</v>
@@ -3294,8 +3314,8 @@
       <c r="A15">
         <v>310</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
+      <c r="B15" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="1">
         <v>0.37809999999999999</v>
@@ -3329,8 +3349,8 @@
       <c r="A16">
         <v>320</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
+      <c r="B16" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="1">
         <v>0.35580000000000001</v>
@@ -3364,8 +3384,8 @@
       <c r="A17">
         <v>330</v>
       </c>
-      <c r="B17" t="s">
-        <v>37</v>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="1">
         <v>0.377</v>
@@ -3399,8 +3419,8 @@
       <c r="A18">
         <v>341</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
+      <c r="B18" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="1">
         <v>0.35339999999999999</v>
@@ -3434,8 +3454,8 @@
       <c r="A19">
         <v>342</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="1">
         <v>0.35339999999999999</v>
@@ -3469,8 +3489,8 @@
       <c r="A20">
         <v>410</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
+      <c r="B20" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C20" s="1">
         <v>0.3881</v>
@@ -3504,8 +3524,8 @@
       <c r="A21">
         <v>420</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
+      <c r="B21" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>0.39639999999999997</v>
@@ -3539,8 +3559,8 @@
       <c r="A22">
         <v>430</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
+      <c r="B22" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C22" s="1">
         <v>0.376</v>
@@ -3574,8 +3594,8 @@
       <c r="A23">
         <v>510</v>
       </c>
-      <c r="B23" t="s">
-        <v>43</v>
+      <c r="B23" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C23" s="1">
         <v>0.39069999999999999</v>
@@ -3609,8 +3629,8 @@
       <c r="A24">
         <v>520</v>
       </c>
-      <c r="B24" t="s">
-        <v>44</v>
+      <c r="B24" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>0.37719999999999998</v>
@@ -3644,8 +3664,8 @@
       <c r="A25">
         <v>530</v>
       </c>
-      <c r="B25" t="s">
-        <v>45</v>
+      <c r="B25" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="C25" s="1">
         <v>0.41</v>
@@ -3679,8 +3699,8 @@
       <c r="A26">
         <v>610</v>
       </c>
-      <c r="B26" t="s">
-        <v>46</v>
+      <c r="B26" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="C26" s="1">
         <v>0.40029999999999999</v>
@@ -3714,8 +3734,8 @@
       <c r="A27">
         <v>620</v>
       </c>
-      <c r="B27" t="s">
-        <v>47</v>
+      <c r="B27" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="C27" s="1">
         <v>0.38540000000000002</v>
@@ -3749,8 +3769,8 @@
       <c r="A28">
         <v>630</v>
       </c>
-      <c r="B28" t="s">
-        <v>48</v>
+      <c r="B28" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C28" s="1">
         <v>0.41510000000000002</v>
@@ -3790,40 +3810,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="C2">
         <v>81</v>
@@ -3839,8 +3859,8 @@
       <c r="A3">
         <v>112</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="C3">
         <v>85</v>
@@ -3856,8 +3876,8 @@
       <c r="A4">
         <v>120</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C4">
         <v>95</v>
@@ -3873,8 +3893,8 @@
       <c r="A5">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
+      <c r="B5" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C5">
         <v>73</v>
@@ -3890,8 +3910,8 @@
       <c r="A6">
         <v>140</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
+      <c r="B6" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C6">
         <v>75</v>
@@ -3907,8 +3927,8 @@
       <c r="A7">
         <v>151</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
+      <c r="B7" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C7">
         <v>58</v>
@@ -3924,8 +3944,8 @@
       <c r="A8">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C8">
         <v>55</v>
@@ -3941,8 +3961,8 @@
       <c r="A9">
         <v>160</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="B9" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="C9">
         <v>52</v>
@@ -3958,8 +3978,8 @@
       <c r="A10">
         <v>170</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
+      <c r="B10" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C10">
         <v>63</v>
@@ -3975,8 +3995,8 @@
       <c r="A11">
         <v>210</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
+      <c r="B11" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C11">
         <v>46</v>
@@ -3992,8 +4012,8 @@
       <c r="A12">
         <v>220</v>
       </c>
-      <c r="B12" t="s">
-        <v>32</v>
+      <c r="B12" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C12">
         <v>49</v>
@@ -4009,8 +4029,8 @@
       <c r="A13">
         <v>230</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
+      <c r="B13" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C13">
         <v>48</v>
@@ -4026,8 +4046,8 @@
       <c r="A14">
         <v>240</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C14">
         <v>48</v>
@@ -4043,8 +4063,8 @@
       <c r="A15">
         <v>310</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
+      <c r="B15" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="C15">
         <v>78</v>
@@ -4060,8 +4080,8 @@
       <c r="A16">
         <v>320</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C16">
         <v>68</v>
@@ -4077,8 +4097,8 @@
       <c r="A17">
         <v>330</v>
       </c>
-      <c r="B17" t="s">
-        <v>37</v>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C17">
         <v>54</v>
@@ -4094,8 +4114,8 @@
       <c r="A18">
         <v>341</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
+      <c r="B18" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C18">
         <v>64</v>
@@ -4111,8 +4131,8 @@
       <c r="A19">
         <v>342</v>
       </c>
-      <c r="B19" t="s">
-        <v>39</v>
+      <c r="B19" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C19">
         <v>68</v>
@@ -4128,8 +4148,8 @@
       <c r="A20">
         <v>410</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
+      <c r="B20" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C20">
         <v>76</v>
@@ -4145,8 +4165,8 @@
       <c r="A21">
         <v>420</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
+      <c r="B21" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C21">
         <v>56</v>
@@ -4162,8 +4182,8 @@
       <c r="A22">
         <v>430</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
+      <c r="B22" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C22">
         <v>65</v>
@@ -4179,8 +4199,8 @@
       <c r="A23">
         <v>510</v>
       </c>
-      <c r="B23" t="s">
-        <v>43</v>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C23">
         <v>48</v>
@@ -4196,8 +4216,8 @@
       <c r="A24">
         <v>520</v>
       </c>
-      <c r="B24" t="s">
-        <v>44</v>
+      <c r="B24" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C24">
         <v>46</v>
@@ -4213,8 +4233,8 @@
       <c r="A25">
         <v>530</v>
       </c>
-      <c r="B25" t="s">
-        <v>45</v>
+      <c r="B25" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C25">
         <v>36</v>
@@ -4230,8 +4250,8 @@
       <c r="A26">
         <v>610</v>
       </c>
-      <c r="B26" t="s">
-        <v>46</v>
+      <c r="B26" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C26">
         <v>68</v>
@@ -4247,8 +4267,8 @@
       <c r="A27">
         <v>620</v>
       </c>
-      <c r="B27" t="s">
-        <v>47</v>
+      <c r="B27" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C27">
         <v>42</v>
@@ -4264,8 +4284,8 @@
       <c r="A28">
         <v>630</v>
       </c>
-      <c r="B28" t="s">
-        <v>48</v>
+      <c r="B28" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C28">
         <v>27</v>

</xml_diff>